<commit_message>
Added Dockerfile for shinyproxy.io
</commit_message>
<xml_diff>
--- a/04-kreise.xlsx
+++ b/04-kreise.xlsx
@@ -19625,8 +19625,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004456E7D0170A5843A32AE86FB4FC254D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="73c0e24160828a1802efa965a6b49054">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0062f6-3850-45c4-a49c-48289d7656f5" xmlns:ns3="d4476a09-aef8-48ac-8c6f-fc751ea8799c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03583cdd2ea035fcfcfa96bf24071983" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004456E7D0170A5843A32AE86FB4FC254D" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="091e3370af739e96a030a0cbf9ddae47">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0062f6-3850-45c4-a49c-48289d7656f5" xmlns:ns3="d4476a09-aef8-48ac-8c6f-fc751ea8799c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edd74138c09f7fd4af0663ac87e10f7f" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0062f6-3850-45c4-a49c-48289d7656f5"/>
     <xsd:import namespace="d4476a09-aef8-48ac-8c6f-fc751ea8799c"/>
     <xsd:element name="properties">
@@ -19646,6 +19646,7 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -19705,11 +19706,16 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d4476a09-aef8-48ac-8c6f-fc751ea8799c" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -19728,7 +19734,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -19745,8 +19751,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -19851,7 +19857,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FFEED42-9C30-431C-92C1-2033691E4568}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C8F6CB3-B8B9-4A0C-B92D-8012B99A5078}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>